<commit_message>
added the figures for distance and learning to the excel sheet
</commit_message>
<xml_diff>
--- a/training_csv_overview/overview_traindyn_favorites.xlsx
+++ b/training_csv_overview/overview_traindyn_favorites.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gt/Documents/GitHub/neural_manifolds/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eghbalhosseini/MyCodes/neural_manifolds/training_csv_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DDA24E-E57E-F84D-BBC3-9761FDADC42E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC85FB6-FCFF-0B45-8D73-3CFE8F3266A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="460" windowWidth="30200" windowHeight="19240" xr2:uid="{57D70428-E33C-FB43-9F81-CF825DE71854}"/>
+    <workbookView xWindow="7320" yWindow="1220" windowWidth="41660" windowHeight="27240" xr2:uid="{57D70428-E33C-FB43-9F81-CF825DE71854}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>lr 0.0005, momentum 0.5, gaussian std 0.0001, batch size 32, 20 epochs</t>
   </si>
@@ -83,12 +74,15 @@
   <si>
     <t>Network #7</t>
   </si>
+  <si>
+    <t>note: some of the distance points are missing(didn’t get analyzed), and the mini spikes in the figure are due to them</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -637,6 +631,138 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>198261</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ADA119A-4702-8941-9C6D-7B83F99C1C71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11633200" y="4102100"/>
+          <a:ext cx="7772400" cy="4833761"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>187547</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F88C389-7967-354E-A376-1BC4388A9A88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11658600" y="9525000"/>
+          <a:ext cx="7772400" cy="4886547"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>152084</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FC171A1-6DD0-7143-A282-4892BD59BE21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14274800" y="25361900"/>
+          <a:ext cx="7772400" cy="4863784"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -937,30 +1063,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B08E62D4-B6AA-6D4B-AA5A-6F10267A87F4}">
-  <dimension ref="A3:Q140"/>
+  <dimension ref="A3:AA153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q126" sqref="A126:Q140"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="R155" sqref="R155"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24">
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+    </row>
+    <row r="21" spans="1:24">
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+    </row>
+    <row r="22" spans="1:24">
       <c r="A22" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+    </row>
+    <row r="23" spans="1:24">
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+    </row>
+    <row r="24" spans="1:24">
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+    </row>
+    <row r="25" spans="1:24">
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+    </row>
+    <row r="26" spans="1:24">
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+    </row>
+    <row r="27" spans="1:24">
       <c r="A27" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+    </row>
+    <row r="28" spans="1:24">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -975,8 +1193,18 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+    </row>
+    <row r="29" spans="1:24">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -993,8 +1221,18 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+    </row>
+    <row r="30" spans="1:24">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1009,8 +1247,18 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+    </row>
+    <row r="31" spans="1:24">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1025,8 +1273,18 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+    </row>
+    <row r="32" spans="1:24">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1041,8 +1299,18 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+    </row>
+    <row r="33" spans="1:24">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1057,8 +1325,18 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+    </row>
+    <row r="34" spans="1:24">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1073,8 +1351,18 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+    </row>
+    <row r="35" spans="1:24">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1089,8 +1377,18 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+    </row>
+    <row r="36" spans="1:24">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1105,8 +1403,18 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+    </row>
+    <row r="37" spans="1:24">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1121,8 +1429,18 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+    </row>
+    <row r="38" spans="1:24">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1137,8 +1455,18 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+    </row>
+    <row r="39" spans="1:24">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1153,8 +1481,18 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+    </row>
+    <row r="40" spans="1:24">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1169,8 +1507,18 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+    </row>
+    <row r="41" spans="1:24">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1185,8 +1533,18 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+    </row>
+    <row r="42" spans="1:24">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1201,8 +1559,18 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+    </row>
+    <row r="43" spans="1:24">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1217,8 +1585,18 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+    </row>
+    <row r="44" spans="1:24">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1233,8 +1611,18 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+    </row>
+    <row r="45" spans="1:24">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1249,13 +1637,25 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+    </row>
+    <row r="46" spans="1:24">
       <c r="A46" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:24">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1270,8 +1670,18 @@
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+    </row>
+    <row r="48" spans="1:24">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1286,8 +1696,18 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+    </row>
+    <row r="49" spans="1:24">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1302,8 +1722,18 @@
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
+      <c r="X49" s="1"/>
+    </row>
+    <row r="50" spans="1:24">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1318,8 +1748,18 @@
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+      <c r="X50" s="1"/>
+    </row>
+    <row r="51" spans="1:24">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1334,8 +1774,18 @@
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+    </row>
+    <row r="52" spans="1:24">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1350,8 +1800,18 @@
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+    </row>
+    <row r="53" spans="1:24">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1366,8 +1826,18 @@
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+    </row>
+    <row r="54" spans="1:24">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1382,8 +1852,18 @@
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="X54" s="1"/>
+    </row>
+    <row r="55" spans="1:24">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1398,8 +1878,18 @@
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
+      <c r="X55" s="1"/>
+    </row>
+    <row r="56" spans="1:24">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1414,8 +1904,18 @@
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+    </row>
+    <row r="57" spans="1:24">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1430,8 +1930,18 @@
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
+      <c r="X57" s="1"/>
+    </row>
+    <row r="58" spans="1:24">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1446,8 +1956,18 @@
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="1"/>
+      <c r="X58" s="1"/>
+    </row>
+    <row r="59" spans="1:24">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1462,8 +1982,18 @@
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
+      <c r="X59" s="1"/>
+    </row>
+    <row r="60" spans="1:24">
       <c r="A60" s="2" t="s">
         <v>2</v>
       </c>
@@ -1482,38 +2012,194 @@
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+      <c r="X60" s="1"/>
+    </row>
+    <row r="61" spans="1:24">
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="1"/>
+      <c r="X61" s="1"/>
+    </row>
+    <row r="62" spans="1:24">
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+      <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="W62" s="1"/>
+      <c r="X62" s="1"/>
+    </row>
+    <row r="63" spans="1:24">
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
+    </row>
+    <row r="64" spans="1:24">
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
+      <c r="X64" s="1"/>
+    </row>
+    <row r="65" spans="1:24">
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="W65" s="1"/>
+      <c r="X65" s="1"/>
+    </row>
+    <row r="66" spans="1:24">
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+    </row>
+    <row r="67" spans="1:24">
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+    </row>
+    <row r="68" spans="1:24">
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+    </row>
+    <row r="69" spans="1:24">
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+    </row>
+    <row r="70" spans="1:24">
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+    </row>
+    <row r="71" spans="1:24">
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+      <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="W71" s="1"/>
+      <c r="X71" s="1"/>
+    </row>
+    <row r="72" spans="1:24">
+      <c r="O72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="1"/>
+      <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
+      <c r="W72" s="1"/>
+      <c r="X72" s="1"/>
+    </row>
+    <row r="76" spans="1:24">
       <c r="A76" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1">
       <c r="A89" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1">
       <c r="A91" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1">
       <c r="A109" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:27">
       <c r="A123" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:27">
       <c r="A125" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:27">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -1531,8 +2217,18 @@
       <c r="O126" s="1"/>
       <c r="P126" s="1"/>
       <c r="Q126" s="1"/>
-    </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R126" s="1"/>
+      <c r="S126" s="1"/>
+      <c r="T126" s="1"/>
+      <c r="U126" s="1"/>
+      <c r="V126" s="1"/>
+      <c r="W126" s="1"/>
+      <c r="X126" s="1"/>
+      <c r="Y126" s="1"/>
+      <c r="Z126" s="1"/>
+      <c r="AA126" s="1"/>
+    </row>
+    <row r="127" spans="1:27">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -1550,8 +2246,18 @@
       <c r="O127" s="1"/>
       <c r="P127" s="1"/>
       <c r="Q127" s="1"/>
-    </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R127" s="1"/>
+      <c r="S127" s="1"/>
+      <c r="T127" s="1"/>
+      <c r="U127" s="1"/>
+      <c r="V127" s="1"/>
+      <c r="W127" s="1"/>
+      <c r="X127" s="1"/>
+      <c r="Y127" s="1"/>
+      <c r="Z127" s="1"/>
+      <c r="AA127" s="1"/>
+    </row>
+    <row r="128" spans="1:27">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -1569,8 +2275,18 @@
       <c r="O128" s="1"/>
       <c r="P128" s="1"/>
       <c r="Q128" s="1"/>
-    </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R128" s="1"/>
+      <c r="S128" s="1"/>
+      <c r="T128" s="1"/>
+      <c r="U128" s="1"/>
+      <c r="V128" s="1"/>
+      <c r="W128" s="1"/>
+      <c r="X128" s="1"/>
+      <c r="Y128" s="1"/>
+      <c r="Z128" s="1"/>
+      <c r="AA128" s="1"/>
+    </row>
+    <row r="129" spans="1:27">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -1588,8 +2304,18 @@
       <c r="O129" s="1"/>
       <c r="P129" s="1"/>
       <c r="Q129" s="1"/>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R129" s="1"/>
+      <c r="S129" s="1"/>
+      <c r="T129" s="1"/>
+      <c r="U129" s="1"/>
+      <c r="V129" s="1"/>
+      <c r="W129" s="1"/>
+      <c r="X129" s="1"/>
+      <c r="Y129" s="1"/>
+      <c r="Z129" s="1"/>
+      <c r="AA129" s="1"/>
+    </row>
+    <row r="130" spans="1:27">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -1607,8 +2333,18 @@
       <c r="O130" s="1"/>
       <c r="P130" s="1"/>
       <c r="Q130" s="1"/>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R130" s="1"/>
+      <c r="S130" s="1"/>
+      <c r="T130" s="1"/>
+      <c r="U130" s="1"/>
+      <c r="V130" s="1"/>
+      <c r="W130" s="1"/>
+      <c r="X130" s="1"/>
+      <c r="Y130" s="1"/>
+      <c r="Z130" s="1"/>
+      <c r="AA130" s="1"/>
+    </row>
+    <row r="131" spans="1:27">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -1626,8 +2362,18 @@
       <c r="O131" s="1"/>
       <c r="P131" s="1"/>
       <c r="Q131" s="1"/>
-    </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R131" s="1"/>
+      <c r="S131" s="1"/>
+      <c r="T131" s="1"/>
+      <c r="U131" s="1"/>
+      <c r="V131" s="1"/>
+      <c r="W131" s="1"/>
+      <c r="X131" s="1"/>
+      <c r="Y131" s="1"/>
+      <c r="Z131" s="1"/>
+      <c r="AA131" s="1"/>
+    </row>
+    <row r="132" spans="1:27">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -1645,8 +2391,18 @@
       <c r="O132" s="1"/>
       <c r="P132" s="1"/>
       <c r="Q132" s="1"/>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R132" s="1"/>
+      <c r="S132" s="1"/>
+      <c r="T132" s="1"/>
+      <c r="U132" s="1"/>
+      <c r="V132" s="1"/>
+      <c r="W132" s="1"/>
+      <c r="X132" s="1"/>
+      <c r="Y132" s="1"/>
+      <c r="Z132" s="1"/>
+      <c r="AA132" s="1"/>
+    </row>
+    <row r="133" spans="1:27">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -1664,8 +2420,18 @@
       <c r="O133" s="1"/>
       <c r="P133" s="1"/>
       <c r="Q133" s="1"/>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R133" s="1"/>
+      <c r="S133" s="1"/>
+      <c r="T133" s="1"/>
+      <c r="U133" s="1"/>
+      <c r="V133" s="1"/>
+      <c r="W133" s="1"/>
+      <c r="X133" s="1"/>
+      <c r="Y133" s="1"/>
+      <c r="Z133" s="1"/>
+      <c r="AA133" s="1"/>
+    </row>
+    <row r="134" spans="1:27">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -1683,8 +2449,18 @@
       <c r="O134" s="1"/>
       <c r="P134" s="1"/>
       <c r="Q134" s="1"/>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R134" s="1"/>
+      <c r="S134" s="1"/>
+      <c r="T134" s="1"/>
+      <c r="U134" s="1"/>
+      <c r="V134" s="1"/>
+      <c r="W134" s="1"/>
+      <c r="X134" s="1"/>
+      <c r="Y134" s="1"/>
+      <c r="Z134" s="1"/>
+      <c r="AA134" s="1"/>
+    </row>
+    <row r="135" spans="1:27">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -1702,8 +2478,18 @@
       <c r="O135" s="1"/>
       <c r="P135" s="1"/>
       <c r="Q135" s="1"/>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R135" s="1"/>
+      <c r="S135" s="1"/>
+      <c r="T135" s="1"/>
+      <c r="U135" s="1"/>
+      <c r="V135" s="1"/>
+      <c r="W135" s="1"/>
+      <c r="X135" s="1"/>
+      <c r="Y135" s="1"/>
+      <c r="Z135" s="1"/>
+      <c r="AA135" s="1"/>
+    </row>
+    <row r="136" spans="1:27">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -1721,8 +2507,18 @@
       <c r="O136" s="1"/>
       <c r="P136" s="1"/>
       <c r="Q136" s="1"/>
-    </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R136" s="1"/>
+      <c r="S136" s="1"/>
+      <c r="T136" s="1"/>
+      <c r="U136" s="1"/>
+      <c r="V136" s="1"/>
+      <c r="W136" s="1"/>
+      <c r="X136" s="1"/>
+      <c r="Y136" s="1"/>
+      <c r="Z136" s="1"/>
+      <c r="AA136" s="1"/>
+    </row>
+    <row r="137" spans="1:27">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -1740,8 +2536,18 @@
       <c r="O137" s="1"/>
       <c r="P137" s="1"/>
       <c r="Q137" s="1"/>
-    </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R137" s="1"/>
+      <c r="S137" s="1"/>
+      <c r="T137" s="1"/>
+      <c r="U137" s="1"/>
+      <c r="V137" s="1"/>
+      <c r="W137" s="1"/>
+      <c r="X137" s="1"/>
+      <c r="Y137" s="1"/>
+      <c r="Z137" s="1"/>
+      <c r="AA137" s="1"/>
+    </row>
+    <row r="138" spans="1:27">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -1759,8 +2565,18 @@
       <c r="O138" s="1"/>
       <c r="P138" s="1"/>
       <c r="Q138" s="1"/>
-    </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R138" s="1"/>
+      <c r="S138" s="1"/>
+      <c r="T138" s="1"/>
+      <c r="U138" s="1"/>
+      <c r="V138" s="1"/>
+      <c r="W138" s="1"/>
+      <c r="X138" s="1"/>
+      <c r="Y138" s="1"/>
+      <c r="Z138" s="1"/>
+      <c r="AA138" s="1"/>
+    </row>
+    <row r="139" spans="1:27">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -1778,8 +2594,18 @@
       <c r="O139" s="1"/>
       <c r="P139" s="1"/>
       <c r="Q139" s="1"/>
-    </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R139" s="1"/>
+      <c r="S139" s="1"/>
+      <c r="T139" s="1"/>
+      <c r="U139" s="1"/>
+      <c r="V139" s="1"/>
+      <c r="W139" s="1"/>
+      <c r="X139" s="1"/>
+      <c r="Y139" s="1"/>
+      <c r="Z139" s="1"/>
+      <c r="AA139" s="1"/>
+    </row>
+    <row r="140" spans="1:27">
       <c r="A140" s="1" t="s">
         <v>9</v>
       </c>
@@ -1803,6 +2629,174 @@
       <c r="O140" s="1"/>
       <c r="P140" s="1"/>
       <c r="Q140" s="1"/>
+      <c r="R140" s="1"/>
+      <c r="S140" s="1"/>
+      <c r="T140" s="1"/>
+      <c r="U140" s="1"/>
+      <c r="V140" s="1"/>
+      <c r="W140" s="1"/>
+      <c r="X140" s="1"/>
+      <c r="Y140" s="1"/>
+      <c r="Z140" s="1"/>
+      <c r="AA140" s="1"/>
+    </row>
+    <row r="141" spans="1:27">
+      <c r="R141" s="1"/>
+      <c r="S141" s="1"/>
+      <c r="T141" s="1"/>
+      <c r="U141" s="1"/>
+      <c r="V141" s="1"/>
+      <c r="W141" s="1"/>
+      <c r="X141" s="1"/>
+      <c r="Y141" s="1"/>
+      <c r="Z141" s="1"/>
+      <c r="AA141" s="1"/>
+    </row>
+    <row r="142" spans="1:27">
+      <c r="R142" s="1"/>
+      <c r="S142" s="1"/>
+      <c r="T142" s="1"/>
+      <c r="U142" s="1"/>
+      <c r="V142" s="1"/>
+      <c r="W142" s="1"/>
+      <c r="X142" s="1"/>
+      <c r="Y142" s="1"/>
+      <c r="Z142" s="1"/>
+      <c r="AA142" s="1"/>
+    </row>
+    <row r="143" spans="1:27">
+      <c r="R143" s="1"/>
+      <c r="S143" s="1"/>
+      <c r="T143" s="1"/>
+      <c r="U143" s="1"/>
+      <c r="V143" s="1"/>
+      <c r="W143" s="1"/>
+      <c r="X143" s="1"/>
+      <c r="Y143" s="1"/>
+      <c r="Z143" s="1"/>
+      <c r="AA143" s="1"/>
+    </row>
+    <row r="144" spans="1:27">
+      <c r="R144" s="1"/>
+      <c r="S144" s="1"/>
+      <c r="T144" s="1"/>
+      <c r="U144" s="1"/>
+      <c r="V144" s="1"/>
+      <c r="W144" s="1"/>
+      <c r="X144" s="1"/>
+      <c r="Y144" s="1"/>
+      <c r="Z144" s="1"/>
+      <c r="AA144" s="1"/>
+    </row>
+    <row r="145" spans="18:27">
+      <c r="R145" s="1"/>
+      <c r="S145" s="1"/>
+      <c r="T145" s="1"/>
+      <c r="U145" s="1"/>
+      <c r="V145" s="1"/>
+      <c r="W145" s="1"/>
+      <c r="X145" s="1"/>
+      <c r="Y145" s="1"/>
+      <c r="Z145" s="1"/>
+      <c r="AA145" s="1"/>
+    </row>
+    <row r="146" spans="18:27">
+      <c r="R146" s="1"/>
+      <c r="S146" s="1"/>
+      <c r="T146" s="1"/>
+      <c r="U146" s="1"/>
+      <c r="V146" s="1"/>
+      <c r="W146" s="1"/>
+      <c r="X146" s="1"/>
+      <c r="Y146" s="1"/>
+      <c r="Z146" s="1"/>
+      <c r="AA146" s="1"/>
+    </row>
+    <row r="147" spans="18:27">
+      <c r="R147" s="1"/>
+      <c r="S147" s="1"/>
+      <c r="T147" s="1"/>
+      <c r="U147" s="1"/>
+      <c r="V147" s="1"/>
+      <c r="W147" s="1"/>
+      <c r="X147" s="1"/>
+      <c r="Y147" s="1"/>
+      <c r="Z147" s="1"/>
+      <c r="AA147" s="1"/>
+    </row>
+    <row r="148" spans="18:27">
+      <c r="R148" s="1"/>
+      <c r="S148" s="1"/>
+      <c r="T148" s="1"/>
+      <c r="U148" s="1"/>
+      <c r="V148" s="1"/>
+      <c r="W148" s="1"/>
+      <c r="X148" s="1"/>
+      <c r="Y148" s="1"/>
+      <c r="Z148" s="1"/>
+      <c r="AA148" s="1"/>
+    </row>
+    <row r="149" spans="18:27">
+      <c r="R149" s="1"/>
+      <c r="S149" s="1"/>
+      <c r="T149" s="1"/>
+      <c r="U149" s="1"/>
+      <c r="V149" s="1"/>
+      <c r="W149" s="1"/>
+      <c r="X149" s="1"/>
+      <c r="Y149" s="1"/>
+      <c r="Z149" s="1"/>
+      <c r="AA149" s="1"/>
+    </row>
+    <row r="150" spans="18:27">
+      <c r="R150" s="1"/>
+      <c r="S150" s="1"/>
+      <c r="T150" s="1"/>
+      <c r="U150" s="1"/>
+      <c r="V150" s="1"/>
+      <c r="W150" s="1"/>
+      <c r="X150" s="1"/>
+      <c r="Y150" s="1"/>
+      <c r="Z150" s="1"/>
+      <c r="AA150" s="1"/>
+    </row>
+    <row r="151" spans="18:27">
+      <c r="R151" s="1"/>
+      <c r="S151" s="1"/>
+      <c r="T151" s="1"/>
+      <c r="U151" s="1"/>
+      <c r="V151" s="1"/>
+      <c r="W151" s="1"/>
+      <c r="X151" s="1"/>
+      <c r="Y151" s="1"/>
+      <c r="Z151" s="1"/>
+      <c r="AA151" s="1"/>
+    </row>
+    <row r="152" spans="18:27">
+      <c r="R152" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S152" s="1"/>
+      <c r="T152" s="1"/>
+      <c r="U152" s="1"/>
+      <c r="V152" s="1"/>
+      <c r="W152" s="1"/>
+      <c r="X152" s="1"/>
+      <c r="Y152" s="1"/>
+      <c r="Z152" s="1"/>
+      <c r="AA152" s="1"/>
+    </row>
+    <row r="153" spans="18:27">
+      <c r="R153" s="1"/>
+      <c r="S153" s="1"/>
+      <c r="T153" s="1"/>
+      <c r="U153" s="1"/>
+      <c r="V153" s="1"/>
+      <c r="W153" s="1"/>
+      <c r="X153" s="1"/>
+      <c r="Y153" s="1"/>
+      <c r="Z153" s="1"/>
+      <c r="AA153" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bugfix, added mftma figure
</commit_message>
<xml_diff>
--- a/training_csv_overview/overview_traindyn_favorites.xlsx
+++ b/training_csv_overview/overview_traindyn_favorites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eghbalhosseini/MyCodes/neural_manifolds/training_csv_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB523F13-1AEA-0A41-BF48-DDADE31723D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0908C01F-C140-824B-9661-9F46D98DF691}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="1220" windowWidth="41660" windowHeight="27240" xr2:uid="{57D70428-E33C-FB43-9F81-CF825DE71854}"/>
+    <workbookView xWindow="-36940" yWindow="2100" windowWidth="36940" windowHeight="21100" xr2:uid="{57D70428-E33C-FB43-9F81-CF825DE71854}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>lr 0.0005, momentum 0.5, gaussian std 0.0001, batch size 32, 20 epochs</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Network #7</t>
-  </si>
-  <si>
-    <t>note: some of the distance points are missing(didn’t get analyzed), and the mini spikes in the figure are due to them</t>
   </si>
 </sst>
 </file>
@@ -633,23 +630,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>198261</xdr:rowOff>
+      <xdr:colOff>790142</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
+        <xdr:cNvPr id="16" name="Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ADA119A-4702-8941-9C6D-7B83F99C1C71}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E823334-69BB-6A47-8A18-55D7392F3D69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -665,8 +662,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11633200" y="4102100"/>
-          <a:ext cx="7772400" cy="4833761"/>
+          <a:off x="11506200" y="3822700"/>
+          <a:ext cx="8270442" cy="5143500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -677,23 +674,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>187547</xdr:rowOff>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>62429</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
+        <xdr:cNvPr id="17" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F88C389-7967-354E-A376-1BC4388A9A88}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97A85977-44A6-9141-ABE1-ECAE74491361}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -709,8 +706,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11658600" y="9525000"/>
-          <a:ext cx="7772400" cy="4886547"/>
+          <a:off x="11442700" y="9283700"/>
+          <a:ext cx="8280400" cy="5205929"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -721,23 +718,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>148</xdr:row>
-      <xdr:rowOff>152084</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>4988</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
+        <xdr:cNvPr id="19" name="Picture 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FC171A1-6DD0-7143-A282-4892BD59BE21}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2DA9083-F468-EB47-8AD0-EADED22E5831}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -753,8 +750,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14274800" y="25361900"/>
-          <a:ext cx="7772400" cy="4863784"/>
+          <a:off x="13817600" y="25387299"/>
+          <a:ext cx="8470900" cy="5300889"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>189470</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4087934-AC22-9B48-A79F-ACB2BD57A8A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20396200" y="2844800"/>
+          <a:ext cx="9690100" cy="6285470"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1063,20 +1104,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B08E62D4-B6AA-6D4B-AA5A-6F10267A87F4}">
-  <dimension ref="A3:AA153"/>
+  <dimension ref="A3:AK153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="R155" sqref="R155"/>
+    <sheetView tabSelected="1" topLeftCell="M12" workbookViewId="0">
+      <selection activeCell="AD55" sqref="AD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="15" spans="1:37">
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1"/>
+    </row>
+    <row r="16" spans="1:37">
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+    </row>
+    <row r="17" spans="1:37">
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1"/>
+    </row>
+    <row r="18" spans="1:37">
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+    </row>
+    <row r="19" spans="1:37">
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+      <c r="AI19" s="1"/>
+      <c r="AJ19" s="1"/>
+      <c r="AK19" s="1"/>
+    </row>
+    <row r="20" spans="1:37">
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -1087,8 +1203,21 @@
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
-    </row>
-    <row r="21" spans="1:24">
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+      <c r="AI20" s="1"/>
+      <c r="AJ20" s="1"/>
+      <c r="AK20" s="1"/>
+    </row>
+    <row r="21" spans="1:37">
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -1099,8 +1228,21 @@
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
-    </row>
-    <row r="22" spans="1:24">
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1"/>
+      <c r="AJ21" s="1"/>
+      <c r="AK21" s="1"/>
+    </row>
+    <row r="22" spans="1:37">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1114,8 +1256,21 @@
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
-    </row>
-    <row r="23" spans="1:24">
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="1"/>
+      <c r="AK22" s="1"/>
+    </row>
+    <row r="23" spans="1:37">
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -1126,8 +1281,21 @@
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
-    </row>
-    <row r="24" spans="1:24">
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1"/>
+      <c r="AI23" s="1"/>
+      <c r="AJ23" s="1"/>
+      <c r="AK23" s="1"/>
+    </row>
+    <row r="24" spans="1:37">
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -1138,8 +1306,21 @@
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
-    </row>
-    <row r="25" spans="1:24">
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1"/>
+      <c r="AI24" s="1"/>
+      <c r="AJ24" s="1"/>
+      <c r="AK24" s="1"/>
+    </row>
+    <row r="25" spans="1:37">
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -1150,8 +1331,21 @@
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
-    </row>
-    <row r="26" spans="1:24">
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AI25" s="1"/>
+      <c r="AJ25" s="1"/>
+      <c r="AK25" s="1"/>
+    </row>
+    <row r="26" spans="1:37">
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
@@ -1162,8 +1356,21 @@
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
-    </row>
-    <row r="27" spans="1:24">
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1"/>
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+      <c r="AI26" s="1"/>
+      <c r="AJ26" s="1"/>
+      <c r="AK26" s="1"/>
+    </row>
+    <row r="27" spans="1:37">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1177,8 +1384,21 @@
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
-    </row>
-    <row r="28" spans="1:24">
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+      <c r="AI27" s="1"/>
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="1"/>
+    </row>
+    <row r="28" spans="1:37">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1203,8 +1423,21 @@
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
-    </row>
-    <row r="29" spans="1:24">
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="1"/>
+      <c r="AJ28" s="1"/>
+      <c r="AK28" s="1"/>
+    </row>
+    <row r="29" spans="1:37">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -1231,8 +1464,21 @@
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
-    </row>
-    <row r="30" spans="1:24">
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+      <c r="AF29" s="1"/>
+      <c r="AG29" s="1"/>
+      <c r="AH29" s="1"/>
+      <c r="AI29" s="1"/>
+      <c r="AJ29" s="1"/>
+      <c r="AK29" s="1"/>
+    </row>
+    <row r="30" spans="1:37">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1257,8 +1503,21 @@
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
-    </row>
-    <row r="31" spans="1:24">
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+      <c r="AF30" s="1"/>
+      <c r="AG30" s="1"/>
+      <c r="AH30" s="1"/>
+      <c r="AI30" s="1"/>
+      <c r="AJ30" s="1"/>
+      <c r="AK30" s="1"/>
+    </row>
+    <row r="31" spans="1:37">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1283,8 +1542,21 @@
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
-    </row>
-    <row r="32" spans="1:24">
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1"/>
+      <c r="AF31" s="1"/>
+      <c r="AG31" s="1"/>
+      <c r="AH31" s="1"/>
+      <c r="AI31" s="1"/>
+      <c r="AJ31" s="1"/>
+      <c r="AK31" s="1"/>
+    </row>
+    <row r="32" spans="1:37">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1309,8 +1581,21 @@
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
-    </row>
-    <row r="33" spans="1:24">
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+      <c r="AF32" s="1"/>
+      <c r="AG32" s="1"/>
+      <c r="AH32" s="1"/>
+      <c r="AI32" s="1"/>
+      <c r="AJ32" s="1"/>
+      <c r="AK32" s="1"/>
+    </row>
+    <row r="33" spans="1:37">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1335,8 +1620,21 @@
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
-    </row>
-    <row r="34" spans="1:24">
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
+      <c r="AF33" s="1"/>
+      <c r="AG33" s="1"/>
+      <c r="AH33" s="1"/>
+      <c r="AI33" s="1"/>
+      <c r="AJ33" s="1"/>
+      <c r="AK33" s="1"/>
+    </row>
+    <row r="34" spans="1:37">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1361,8 +1659,21 @@
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
-    </row>
-    <row r="35" spans="1:24">
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+      <c r="AF34" s="1"/>
+      <c r="AG34" s="1"/>
+      <c r="AH34" s="1"/>
+      <c r="AI34" s="1"/>
+      <c r="AJ34" s="1"/>
+      <c r="AK34" s="1"/>
+    </row>
+    <row r="35" spans="1:37">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1387,8 +1698,21 @@
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
-    </row>
-    <row r="36" spans="1:24">
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="1"/>
+      <c r="AC35" s="1"/>
+      <c r="AD35" s="1"/>
+      <c r="AE35" s="1"/>
+      <c r="AF35" s="1"/>
+      <c r="AG35" s="1"/>
+      <c r="AH35" s="1"/>
+      <c r="AI35" s="1"/>
+      <c r="AJ35" s="1"/>
+      <c r="AK35" s="1"/>
+    </row>
+    <row r="36" spans="1:37">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1413,8 +1737,21 @@
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
-    </row>
-    <row r="37" spans="1:24">
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
+      <c r="AF36" s="1"/>
+      <c r="AG36" s="1"/>
+      <c r="AH36" s="1"/>
+      <c r="AI36" s="1"/>
+      <c r="AJ36" s="1"/>
+      <c r="AK36" s="1"/>
+    </row>
+    <row r="37" spans="1:37">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1439,8 +1776,21 @@
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
-    </row>
-    <row r="38" spans="1:24">
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="1"/>
+      <c r="AC37" s="1"/>
+      <c r="AD37" s="1"/>
+      <c r="AE37" s="1"/>
+      <c r="AF37" s="1"/>
+      <c r="AG37" s="1"/>
+      <c r="AH37" s="1"/>
+      <c r="AI37" s="1"/>
+      <c r="AJ37" s="1"/>
+      <c r="AK37" s="1"/>
+    </row>
+    <row r="38" spans="1:37">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1465,8 +1815,21 @@
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
-    </row>
-    <row r="39" spans="1:24">
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="1"/>
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="1"/>
+      <c r="AG38" s="1"/>
+      <c r="AH38" s="1"/>
+      <c r="AI38" s="1"/>
+      <c r="AJ38" s="1"/>
+      <c r="AK38" s="1"/>
+    </row>
+    <row r="39" spans="1:37">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1491,8 +1854,21 @@
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
-    </row>
-    <row r="40" spans="1:24">
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1"/>
+      <c r="AB39" s="1"/>
+      <c r="AC39" s="1"/>
+      <c r="AD39" s="1"/>
+      <c r="AE39" s="1"/>
+      <c r="AF39" s="1"/>
+      <c r="AG39" s="1"/>
+      <c r="AH39" s="1"/>
+      <c r="AI39" s="1"/>
+      <c r="AJ39" s="1"/>
+      <c r="AK39" s="1"/>
+    </row>
+    <row r="40" spans="1:37">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1517,8 +1893,21 @@
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
-    </row>
-    <row r="41" spans="1:24">
+      <c r="Y40" s="1"/>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
+      <c r="AB40" s="1"/>
+      <c r="AC40" s="1"/>
+      <c r="AD40" s="1"/>
+      <c r="AE40" s="1"/>
+      <c r="AF40" s="1"/>
+      <c r="AG40" s="1"/>
+      <c r="AH40" s="1"/>
+      <c r="AI40" s="1"/>
+      <c r="AJ40" s="1"/>
+      <c r="AK40" s="1"/>
+    </row>
+    <row r="41" spans="1:37">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1543,8 +1932,21 @@
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
-    </row>
-    <row r="42" spans="1:24">
+      <c r="Y41" s="1"/>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1"/>
+      <c r="AB41" s="1"/>
+      <c r="AC41" s="1"/>
+      <c r="AD41" s="1"/>
+      <c r="AE41" s="1"/>
+      <c r="AF41" s="1"/>
+      <c r="AG41" s="1"/>
+      <c r="AH41" s="1"/>
+      <c r="AI41" s="1"/>
+      <c r="AJ41" s="1"/>
+      <c r="AK41" s="1"/>
+    </row>
+    <row r="42" spans="1:37">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1569,8 +1971,21 @@
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
-    </row>
-    <row r="43" spans="1:24">
+      <c r="Y42" s="1"/>
+      <c r="Z42" s="1"/>
+      <c r="AA42" s="1"/>
+      <c r="AB42" s="1"/>
+      <c r="AC42" s="1"/>
+      <c r="AD42" s="1"/>
+      <c r="AE42" s="1"/>
+      <c r="AF42" s="1"/>
+      <c r="AG42" s="1"/>
+      <c r="AH42" s="1"/>
+      <c r="AI42" s="1"/>
+      <c r="AJ42" s="1"/>
+      <c r="AK42" s="1"/>
+    </row>
+    <row r="43" spans="1:37">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1595,8 +2010,21 @@
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
-    </row>
-    <row r="44" spans="1:24">
+      <c r="Y43" s="1"/>
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="1"/>
+      <c r="AB43" s="1"/>
+      <c r="AC43" s="1"/>
+      <c r="AD43" s="1"/>
+      <c r="AE43" s="1"/>
+      <c r="AF43" s="1"/>
+      <c r="AG43" s="1"/>
+      <c r="AH43" s="1"/>
+      <c r="AI43" s="1"/>
+      <c r="AJ43" s="1"/>
+      <c r="AK43" s="1"/>
+    </row>
+    <row r="44" spans="1:37">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1621,8 +2049,21 @@
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
-    </row>
-    <row r="45" spans="1:24">
+      <c r="Y44" s="1"/>
+      <c r="Z44" s="1"/>
+      <c r="AA44" s="1"/>
+      <c r="AB44" s="1"/>
+      <c r="AC44" s="1"/>
+      <c r="AD44" s="1"/>
+      <c r="AE44" s="1"/>
+      <c r="AF44" s="1"/>
+      <c r="AG44" s="1"/>
+      <c r="AH44" s="1"/>
+      <c r="AI44" s="1"/>
+      <c r="AJ44" s="1"/>
+      <c r="AK44" s="1"/>
+    </row>
+    <row r="45" spans="1:37">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1637,9 +2078,7 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
-      <c r="O45" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="O45" s="1"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
@@ -1649,13 +2088,26 @@
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
-    </row>
-    <row r="46" spans="1:24">
+      <c r="Y45" s="1"/>
+      <c r="Z45" s="1"/>
+      <c r="AA45" s="1"/>
+      <c r="AB45" s="1"/>
+      <c r="AC45" s="1"/>
+      <c r="AD45" s="1"/>
+      <c r="AE45" s="1"/>
+      <c r="AF45" s="1"/>
+      <c r="AG45" s="1"/>
+      <c r="AH45" s="1"/>
+      <c r="AI45" s="1"/>
+      <c r="AJ45" s="1"/>
+      <c r="AK45" s="1"/>
+    </row>
+    <row r="46" spans="1:37">
       <c r="A46" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:24">
+    <row r="47" spans="1:37">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1681,7 +2133,7 @@
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
     </row>
-    <row r="48" spans="1:24">
+    <row r="48" spans="1:37">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2156,9 +2608,7 @@
       <c r="X71" s="1"/>
     </row>
     <row r="72" spans="1:24">
-      <c r="O72" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="O72" s="1"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
@@ -2773,9 +3223,7 @@
       <c r="AA151" s="1"/>
     </row>
     <row r="152" spans="18:27">
-      <c r="R152" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="R152" s="1"/>
       <c r="S152" s="1"/>
       <c r="T152" s="1"/>
       <c r="U152" s="1"/>

</xml_diff>

<commit_message>
update for mftma results,
</commit_message>
<xml_diff>
--- a/training_csv_overview/overview_traindyn_favorites.xlsx
+++ b/training_csv_overview/overview_traindyn_favorites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eghbalhosseini/MyCodes/neural_manifolds/training_csv_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0908C01F-C140-824B-9661-9F46D98DF691}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B98021E-08B5-FA4C-ACDF-795AF67FE57E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36940" yWindow="2100" windowWidth="36940" windowHeight="21100" xr2:uid="{57D70428-E33C-FB43-9F81-CF825DE71854}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -631,22 +631,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
+      <xdr:colOff>787399</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>790142</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>242812</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15">
+        <xdr:cNvPr id="14" name="Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E823334-69BB-6A47-8A18-55D7392F3D69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0363862-B1D3-B146-AB75-D15DD9BC6149}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -662,8 +662,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11506200" y="3822700"/>
-          <a:ext cx="8270442" cy="5143500"/>
+          <a:off x="11518899" y="3797300"/>
+          <a:ext cx="8535913" cy="5308600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -674,23 +674,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>62429</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>34324</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
+        <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97A85977-44A6-9141-ABE1-ECAE74491361}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96274132-F21A-0149-A49A-82D6EBBF3A87}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -706,8 +706,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11442700" y="9283700"/>
-          <a:ext cx="8280400" cy="5205929"/>
+          <a:off x="20193000" y="3098800"/>
+          <a:ext cx="9372600" cy="6079524"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -718,23 +718,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>124</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>151</xdr:row>
-      <xdr:rowOff>4988</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>216406</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18">
+        <xdr:cNvPr id="18" name="Picture 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2DA9083-F468-EB47-8AD0-EADED22E5831}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD73F178-A670-0242-90C5-AD385C0F984C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -750,8 +750,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13817600" y="25387299"/>
-          <a:ext cx="8470900" cy="5300889"/>
+          <a:off x="11544300" y="9398000"/>
+          <a:ext cx="8484106" cy="5334000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -763,22 +763,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>189470</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>99197</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
+        <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4087934-AC22-9B48-A79F-ACB2BD57A8A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4D8664E-6C49-334E-8807-4B00BABF7823}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -794,8 +794,96 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20396200" y="2844800"/>
-          <a:ext cx="9690100" cy="6285470"/>
+          <a:off x="20307300" y="9309099"/>
+          <a:ext cx="9296400" cy="6030098"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>596212</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>517528</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>120135</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DF593B8-A035-4940-998B-E55C48DDE75A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13776753" y="25715097"/>
+          <a:ext cx="8982937" cy="5708822"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>669324</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>34323</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>629176</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>85809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54535780-9A73-5740-A2DD-92E92311E67D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22911486" y="25777566"/>
+          <a:ext cx="9845258" cy="6435811"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1104,20 +1192,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B08E62D4-B6AA-6D4B-AA5A-6F10267A87F4}">
-  <dimension ref="A3:AK153"/>
+  <dimension ref="A3:AN156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M12" workbookViewId="0">
-      <selection activeCell="AD55" sqref="AD55"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="AK161" sqref="AK161"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
@@ -1132,7 +1220,7 @@
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
@@ -1147,7 +1235,7 @@
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
@@ -1162,7 +1250,7 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
@@ -1177,7 +1265,7 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
@@ -1192,7 +1280,7 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -1217,7 +1305,7 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -1242,7 +1330,7 @@
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1270,7 +1358,7 @@
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -1295,7 +1383,7 @@
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -1320,7 +1408,7 @@
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -1345,7 +1433,7 @@
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
@@ -1370,7 +1458,7 @@
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1398,7 +1486,7 @@
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1437,7 +1525,7 @@
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -1478,7 +1566,7 @@
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1517,7 +1605,7 @@
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1556,7 +1644,7 @@
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1595,7 +1683,7 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1634,7 +1722,7 @@
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1673,7 +1761,7 @@
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
     </row>
-    <row r="35" spans="1:37">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1712,7 +1800,7 @@
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1751,7 +1839,7 @@
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
     </row>
-    <row r="37" spans="1:37">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1790,7 +1878,7 @@
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1829,7 +1917,7 @@
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1868,7 +1956,7 @@
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1907,7 +1995,7 @@
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
     </row>
-    <row r="41" spans="1:37">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1946,7 +2034,7 @@
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
     </row>
-    <row r="42" spans="1:37">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1985,7 +2073,7 @@
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
     </row>
-    <row r="43" spans="1:37">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2024,7 +2112,7 @@
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1"/>
     </row>
-    <row r="44" spans="1:37">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2063,7 +2151,7 @@
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
     </row>
-    <row r="45" spans="1:37">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2102,12 +2190,12 @@
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
     </row>
-    <row r="46" spans="1:37">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2132,8 +2220,21 @@
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
-    </row>
-    <row r="48" spans="1:37">
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1"/>
+      <c r="AA47" s="1"/>
+      <c r="AB47" s="1"/>
+      <c r="AC47" s="1"/>
+      <c r="AD47" s="1"/>
+      <c r="AE47" s="1"/>
+      <c r="AF47" s="1"/>
+      <c r="AG47" s="1"/>
+      <c r="AH47" s="1"/>
+      <c r="AI47" s="1"/>
+      <c r="AJ47" s="1"/>
+      <c r="AK47" s="1"/>
+    </row>
+    <row r="48" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2158,8 +2259,21 @@
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
-    </row>
-    <row r="49" spans="1:24">
+      <c r="Y48" s="1"/>
+      <c r="Z48" s="1"/>
+      <c r="AA48" s="1"/>
+      <c r="AB48" s="1"/>
+      <c r="AC48" s="1"/>
+      <c r="AD48" s="1"/>
+      <c r="AE48" s="1"/>
+      <c r="AF48" s="1"/>
+      <c r="AG48" s="1"/>
+      <c r="AH48" s="1"/>
+      <c r="AI48" s="1"/>
+      <c r="AJ48" s="1"/>
+      <c r="AK48" s="1"/>
+    </row>
+    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2184,8 +2298,21 @@
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
-    </row>
-    <row r="50" spans="1:24">
+      <c r="Y49" s="1"/>
+      <c r="Z49" s="1"/>
+      <c r="AA49" s="1"/>
+      <c r="AB49" s="1"/>
+      <c r="AC49" s="1"/>
+      <c r="AD49" s="1"/>
+      <c r="AE49" s="1"/>
+      <c r="AF49" s="1"/>
+      <c r="AG49" s="1"/>
+      <c r="AH49" s="1"/>
+      <c r="AI49" s="1"/>
+      <c r="AJ49" s="1"/>
+      <c r="AK49" s="1"/>
+    </row>
+    <row r="50" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2210,8 +2337,21 @@
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
-    </row>
-    <row r="51" spans="1:24">
+      <c r="Y50" s="1"/>
+      <c r="Z50" s="1"/>
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="1"/>
+      <c r="AC50" s="1"/>
+      <c r="AD50" s="1"/>
+      <c r="AE50" s="1"/>
+      <c r="AF50" s="1"/>
+      <c r="AG50" s="1"/>
+      <c r="AH50" s="1"/>
+      <c r="AI50" s="1"/>
+      <c r="AJ50" s="1"/>
+      <c r="AK50" s="1"/>
+    </row>
+    <row r="51" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2236,8 +2376,21 @@
       <c r="V51" s="1"/>
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
-    </row>
-    <row r="52" spans="1:24">
+      <c r="Y51" s="1"/>
+      <c r="Z51" s="1"/>
+      <c r="AA51" s="1"/>
+      <c r="AB51" s="1"/>
+      <c r="AC51" s="1"/>
+      <c r="AD51" s="1"/>
+      <c r="AE51" s="1"/>
+      <c r="AF51" s="1"/>
+      <c r="AG51" s="1"/>
+      <c r="AH51" s="1"/>
+      <c r="AI51" s="1"/>
+      <c r="AJ51" s="1"/>
+      <c r="AK51" s="1"/>
+    </row>
+    <row r="52" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2262,8 +2415,21 @@
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
       <c r="X52" s="1"/>
-    </row>
-    <row r="53" spans="1:24">
+      <c r="Y52" s="1"/>
+      <c r="Z52" s="1"/>
+      <c r="AA52" s="1"/>
+      <c r="AB52" s="1"/>
+      <c r="AC52" s="1"/>
+      <c r="AD52" s="1"/>
+      <c r="AE52" s="1"/>
+      <c r="AF52" s="1"/>
+      <c r="AG52" s="1"/>
+      <c r="AH52" s="1"/>
+      <c r="AI52" s="1"/>
+      <c r="AJ52" s="1"/>
+      <c r="AK52" s="1"/>
+    </row>
+    <row r="53" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2288,8 +2454,21 @@
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
-    </row>
-    <row r="54" spans="1:24">
+      <c r="Y53" s="1"/>
+      <c r="Z53" s="1"/>
+      <c r="AA53" s="1"/>
+      <c r="AB53" s="1"/>
+      <c r="AC53" s="1"/>
+      <c r="AD53" s="1"/>
+      <c r="AE53" s="1"/>
+      <c r="AF53" s="1"/>
+      <c r="AG53" s="1"/>
+      <c r="AH53" s="1"/>
+      <c r="AI53" s="1"/>
+      <c r="AJ53" s="1"/>
+      <c r="AK53" s="1"/>
+    </row>
+    <row r="54" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2314,8 +2493,21 @@
       <c r="V54" s="1"/>
       <c r="W54" s="1"/>
       <c r="X54" s="1"/>
-    </row>
-    <row r="55" spans="1:24">
+      <c r="Y54" s="1"/>
+      <c r="Z54" s="1"/>
+      <c r="AA54" s="1"/>
+      <c r="AB54" s="1"/>
+      <c r="AC54" s="1"/>
+      <c r="AD54" s="1"/>
+      <c r="AE54" s="1"/>
+      <c r="AF54" s="1"/>
+      <c r="AG54" s="1"/>
+      <c r="AH54" s="1"/>
+      <c r="AI54" s="1"/>
+      <c r="AJ54" s="1"/>
+      <c r="AK54" s="1"/>
+    </row>
+    <row r="55" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2340,8 +2532,21 @@
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
       <c r="X55" s="1"/>
-    </row>
-    <row r="56" spans="1:24">
+      <c r="Y55" s="1"/>
+      <c r="Z55" s="1"/>
+      <c r="AA55" s="1"/>
+      <c r="AB55" s="1"/>
+      <c r="AC55" s="1"/>
+      <c r="AD55" s="1"/>
+      <c r="AE55" s="1"/>
+      <c r="AF55" s="1"/>
+      <c r="AG55" s="1"/>
+      <c r="AH55" s="1"/>
+      <c r="AI55" s="1"/>
+      <c r="AJ55" s="1"/>
+      <c r="AK55" s="1"/>
+    </row>
+    <row r="56" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2366,8 +2571,21 @@
       <c r="V56" s="1"/>
       <c r="W56" s="1"/>
       <c r="X56" s="1"/>
-    </row>
-    <row r="57" spans="1:24">
+      <c r="Y56" s="1"/>
+      <c r="Z56" s="1"/>
+      <c r="AA56" s="1"/>
+      <c r="AB56" s="1"/>
+      <c r="AC56" s="1"/>
+      <c r="AD56" s="1"/>
+      <c r="AE56" s="1"/>
+      <c r="AF56" s="1"/>
+      <c r="AG56" s="1"/>
+      <c r="AH56" s="1"/>
+      <c r="AI56" s="1"/>
+      <c r="AJ56" s="1"/>
+      <c r="AK56" s="1"/>
+    </row>
+    <row r="57" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2392,8 +2610,21 @@
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
-    </row>
-    <row r="58" spans="1:24">
+      <c r="Y57" s="1"/>
+      <c r="Z57" s="1"/>
+      <c r="AA57" s="1"/>
+      <c r="AB57" s="1"/>
+      <c r="AC57" s="1"/>
+      <c r="AD57" s="1"/>
+      <c r="AE57" s="1"/>
+      <c r="AF57" s="1"/>
+      <c r="AG57" s="1"/>
+      <c r="AH57" s="1"/>
+      <c r="AI57" s="1"/>
+      <c r="AJ57" s="1"/>
+      <c r="AK57" s="1"/>
+    </row>
+    <row r="58" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2418,8 +2649,21 @@
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
       <c r="X58" s="1"/>
-    </row>
-    <row r="59" spans="1:24">
+      <c r="Y58" s="1"/>
+      <c r="Z58" s="1"/>
+      <c r="AA58" s="1"/>
+      <c r="AB58" s="1"/>
+      <c r="AC58" s="1"/>
+      <c r="AD58" s="1"/>
+      <c r="AE58" s="1"/>
+      <c r="AF58" s="1"/>
+      <c r="AG58" s="1"/>
+      <c r="AH58" s="1"/>
+      <c r="AI58" s="1"/>
+      <c r="AJ58" s="1"/>
+      <c r="AK58" s="1"/>
+    </row>
+    <row r="59" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2444,8 +2688,21 @@
       <c r="V59" s="1"/>
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
-    </row>
-    <row r="60" spans="1:24">
+      <c r="Y59" s="1"/>
+      <c r="Z59" s="1"/>
+      <c r="AA59" s="1"/>
+      <c r="AB59" s="1"/>
+      <c r="AC59" s="1"/>
+      <c r="AD59" s="1"/>
+      <c r="AE59" s="1"/>
+      <c r="AF59" s="1"/>
+      <c r="AG59" s="1"/>
+      <c r="AH59" s="1"/>
+      <c r="AI59" s="1"/>
+      <c r="AJ59" s="1"/>
+      <c r="AK59" s="1"/>
+    </row>
+    <row r="60" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>2</v>
       </c>
@@ -2474,8 +2731,21 @@
       <c r="V60" s="1"/>
       <c r="W60" s="1"/>
       <c r="X60" s="1"/>
-    </row>
-    <row r="61" spans="1:24">
+      <c r="Y60" s="1"/>
+      <c r="Z60" s="1"/>
+      <c r="AA60" s="1"/>
+      <c r="AB60" s="1"/>
+      <c r="AC60" s="1"/>
+      <c r="AD60" s="1"/>
+      <c r="AE60" s="1"/>
+      <c r="AF60" s="1"/>
+      <c r="AG60" s="1"/>
+      <c r="AH60" s="1"/>
+      <c r="AI60" s="1"/>
+      <c r="AJ60" s="1"/>
+      <c r="AK60" s="1"/>
+    </row>
+    <row r="61" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
@@ -2486,8 +2756,21 @@
       <c r="V61" s="1"/>
       <c r="W61" s="1"/>
       <c r="X61" s="1"/>
-    </row>
-    <row r="62" spans="1:24">
+      <c r="Y61" s="1"/>
+      <c r="Z61" s="1"/>
+      <c r="AA61" s="1"/>
+      <c r="AB61" s="1"/>
+      <c r="AC61" s="1"/>
+      <c r="AD61" s="1"/>
+      <c r="AE61" s="1"/>
+      <c r="AF61" s="1"/>
+      <c r="AG61" s="1"/>
+      <c r="AH61" s="1"/>
+      <c r="AI61" s="1"/>
+      <c r="AJ61" s="1"/>
+      <c r="AK61" s="1"/>
+    </row>
+    <row r="62" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
@@ -2498,8 +2781,21 @@
       <c r="V62" s="1"/>
       <c r="W62" s="1"/>
       <c r="X62" s="1"/>
-    </row>
-    <row r="63" spans="1:24">
+      <c r="Y62" s="1"/>
+      <c r="Z62" s="1"/>
+      <c r="AA62" s="1"/>
+      <c r="AB62" s="1"/>
+      <c r="AC62" s="1"/>
+      <c r="AD62" s="1"/>
+      <c r="AE62" s="1"/>
+      <c r="AF62" s="1"/>
+      <c r="AG62" s="1"/>
+      <c r="AH62" s="1"/>
+      <c r="AI62" s="1"/>
+      <c r="AJ62" s="1"/>
+      <c r="AK62" s="1"/>
+    </row>
+    <row r="63" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
@@ -2510,8 +2806,21 @@
       <c r="V63" s="1"/>
       <c r="W63" s="1"/>
       <c r="X63" s="1"/>
-    </row>
-    <row r="64" spans="1:24">
+      <c r="Y63" s="1"/>
+      <c r="Z63" s="1"/>
+      <c r="AA63" s="1"/>
+      <c r="AB63" s="1"/>
+      <c r="AC63" s="1"/>
+      <c r="AD63" s="1"/>
+      <c r="AE63" s="1"/>
+      <c r="AF63" s="1"/>
+      <c r="AG63" s="1"/>
+      <c r="AH63" s="1"/>
+      <c r="AI63" s="1"/>
+      <c r="AJ63" s="1"/>
+      <c r="AK63" s="1"/>
+    </row>
+    <row r="64" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
@@ -2522,8 +2831,21 @@
       <c r="V64" s="1"/>
       <c r="W64" s="1"/>
       <c r="X64" s="1"/>
-    </row>
-    <row r="65" spans="1:24">
+      <c r="Y64" s="1"/>
+      <c r="Z64" s="1"/>
+      <c r="AA64" s="1"/>
+      <c r="AB64" s="1"/>
+      <c r="AC64" s="1"/>
+      <c r="AD64" s="1"/>
+      <c r="AE64" s="1"/>
+      <c r="AF64" s="1"/>
+      <c r="AG64" s="1"/>
+      <c r="AH64" s="1"/>
+      <c r="AI64" s="1"/>
+      <c r="AJ64" s="1"/>
+      <c r="AK64" s="1"/>
+    </row>
+    <row r="65" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
@@ -2534,8 +2856,21 @@
       <c r="V65" s="1"/>
       <c r="W65" s="1"/>
       <c r="X65" s="1"/>
-    </row>
-    <row r="66" spans="1:24">
+      <c r="Y65" s="1"/>
+      <c r="Z65" s="1"/>
+      <c r="AA65" s="1"/>
+      <c r="AB65" s="1"/>
+      <c r="AC65" s="1"/>
+      <c r="AD65" s="1"/>
+      <c r="AE65" s="1"/>
+      <c r="AF65" s="1"/>
+      <c r="AG65" s="1"/>
+      <c r="AH65" s="1"/>
+      <c r="AI65" s="1"/>
+      <c r="AJ65" s="1"/>
+      <c r="AK65" s="1"/>
+    </row>
+    <row r="66" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
@@ -2546,8 +2881,21 @@
       <c r="V66" s="1"/>
       <c r="W66" s="1"/>
       <c r="X66" s="1"/>
-    </row>
-    <row r="67" spans="1:24">
+      <c r="Y66" s="1"/>
+      <c r="Z66" s="1"/>
+      <c r="AA66" s="1"/>
+      <c r="AB66" s="1"/>
+      <c r="AC66" s="1"/>
+      <c r="AD66" s="1"/>
+      <c r="AE66" s="1"/>
+      <c r="AF66" s="1"/>
+      <c r="AG66" s="1"/>
+      <c r="AH66" s="1"/>
+      <c r="AI66" s="1"/>
+      <c r="AJ66" s="1"/>
+      <c r="AK66" s="1"/>
+    </row>
+    <row r="67" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
@@ -2558,8 +2906,21 @@
       <c r="V67" s="1"/>
       <c r="W67" s="1"/>
       <c r="X67" s="1"/>
-    </row>
-    <row r="68" spans="1:24">
+      <c r="Y67" s="1"/>
+      <c r="Z67" s="1"/>
+      <c r="AA67" s="1"/>
+      <c r="AB67" s="1"/>
+      <c r="AC67" s="1"/>
+      <c r="AD67" s="1"/>
+      <c r="AE67" s="1"/>
+      <c r="AF67" s="1"/>
+      <c r="AG67" s="1"/>
+      <c r="AH67" s="1"/>
+      <c r="AI67" s="1"/>
+      <c r="AJ67" s="1"/>
+      <c r="AK67" s="1"/>
+    </row>
+    <row r="68" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
@@ -2570,8 +2931,21 @@
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
       <c r="X68" s="1"/>
-    </row>
-    <row r="69" spans="1:24">
+      <c r="Y68" s="1"/>
+      <c r="Z68" s="1"/>
+      <c r="AA68" s="1"/>
+      <c r="AB68" s="1"/>
+      <c r="AC68" s="1"/>
+      <c r="AD68" s="1"/>
+      <c r="AE68" s="1"/>
+      <c r="AF68" s="1"/>
+      <c r="AG68" s="1"/>
+      <c r="AH68" s="1"/>
+      <c r="AI68" s="1"/>
+      <c r="AJ68" s="1"/>
+      <c r="AK68" s="1"/>
+    </row>
+    <row r="69" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
@@ -2582,8 +2956,21 @@
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
       <c r="X69" s="1"/>
-    </row>
-    <row r="70" spans="1:24">
+      <c r="Y69" s="1"/>
+      <c r="Z69" s="1"/>
+      <c r="AA69" s="1"/>
+      <c r="AB69" s="1"/>
+      <c r="AC69" s="1"/>
+      <c r="AD69" s="1"/>
+      <c r="AE69" s="1"/>
+      <c r="AF69" s="1"/>
+      <c r="AG69" s="1"/>
+      <c r="AH69" s="1"/>
+      <c r="AI69" s="1"/>
+      <c r="AJ69" s="1"/>
+      <c r="AK69" s="1"/>
+    </row>
+    <row r="70" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
@@ -2594,8 +2981,21 @@
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
       <c r="X70" s="1"/>
-    </row>
-    <row r="71" spans="1:24">
+      <c r="Y70" s="1"/>
+      <c r="Z70" s="1"/>
+      <c r="AA70" s="1"/>
+      <c r="AB70" s="1"/>
+      <c r="AC70" s="1"/>
+      <c r="AD70" s="1"/>
+      <c r="AE70" s="1"/>
+      <c r="AF70" s="1"/>
+      <c r="AG70" s="1"/>
+      <c r="AH70" s="1"/>
+      <c r="AI70" s="1"/>
+      <c r="AJ70" s="1"/>
+      <c r="AK70" s="1"/>
+    </row>
+    <row r="71" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
@@ -2606,8 +3006,21 @@
       <c r="V71" s="1"/>
       <c r="W71" s="1"/>
       <c r="X71" s="1"/>
-    </row>
-    <row r="72" spans="1:24">
+      <c r="Y71" s="1"/>
+      <c r="Z71" s="1"/>
+      <c r="AA71" s="1"/>
+      <c r="AB71" s="1"/>
+      <c r="AC71" s="1"/>
+      <c r="AD71" s="1"/>
+      <c r="AE71" s="1"/>
+      <c r="AF71" s="1"/>
+      <c r="AG71" s="1"/>
+      <c r="AH71" s="1"/>
+      <c r="AI71" s="1"/>
+      <c r="AJ71" s="1"/>
+      <c r="AK71" s="1"/>
+    </row>
+    <row r="72" spans="1:37" x14ac:dyDescent="0.2">
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
@@ -2618,38 +3031,119 @@
       <c r="V72" s="1"/>
       <c r="W72" s="1"/>
       <c r="X72" s="1"/>
-    </row>
-    <row r="76" spans="1:24">
+      <c r="Y72" s="1"/>
+      <c r="Z72" s="1"/>
+      <c r="AA72" s="1"/>
+      <c r="AB72" s="1"/>
+      <c r="AC72" s="1"/>
+      <c r="AD72" s="1"/>
+      <c r="AE72" s="1"/>
+      <c r="AF72" s="1"/>
+      <c r="AG72" s="1"/>
+      <c r="AH72" s="1"/>
+      <c r="AI72" s="1"/>
+      <c r="AJ72" s="1"/>
+      <c r="AK72" s="1"/>
+    </row>
+    <row r="73" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1"/>
+      <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
+      <c r="W73" s="1"/>
+      <c r="X73" s="1"/>
+      <c r="Y73" s="1"/>
+      <c r="Z73" s="1"/>
+      <c r="AA73" s="1"/>
+      <c r="AB73" s="1"/>
+      <c r="AC73" s="1"/>
+      <c r="AD73" s="1"/>
+      <c r="AE73" s="1"/>
+      <c r="AF73" s="1"/>
+      <c r="AG73" s="1"/>
+      <c r="AH73" s="1"/>
+      <c r="AI73" s="1"/>
+      <c r="AJ73" s="1"/>
+      <c r="AK73" s="1"/>
+    </row>
+    <row r="74" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Y74" s="1"/>
+      <c r="Z74" s="1"/>
+      <c r="AA74" s="1"/>
+      <c r="AB74" s="1"/>
+      <c r="AC74" s="1"/>
+      <c r="AD74" s="1"/>
+      <c r="AE74" s="1"/>
+      <c r="AF74" s="1"/>
+      <c r="AG74" s="1"/>
+      <c r="AH74" s="1"/>
+      <c r="AI74" s="1"/>
+      <c r="AJ74" s="1"/>
+      <c r="AK74" s="1"/>
+    </row>
+    <row r="75" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Y75" s="1"/>
+      <c r="Z75" s="1"/>
+      <c r="AA75" s="1"/>
+      <c r="AB75" s="1"/>
+      <c r="AC75" s="1"/>
+      <c r="AD75" s="1"/>
+      <c r="AE75" s="1"/>
+      <c r="AF75" s="1"/>
+      <c r="AG75" s="1"/>
+      <c r="AH75" s="1"/>
+      <c r="AI75" s="1"/>
+      <c r="AJ75" s="1"/>
+      <c r="AK75" s="1"/>
+    </row>
+    <row r="76" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="89" spans="1:1">
+      <c r="Y76" s="1"/>
+      <c r="Z76" s="1"/>
+      <c r="AA76" s="1"/>
+      <c r="AB76" s="1"/>
+      <c r="AC76" s="1"/>
+      <c r="AD76" s="1"/>
+      <c r="AE76" s="1"/>
+      <c r="AF76" s="1"/>
+      <c r="AG76" s="1"/>
+      <c r="AH76" s="1"/>
+      <c r="AI76" s="1"/>
+      <c r="AJ76" s="1"/>
+      <c r="AK76" s="1"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:27">
+    <row r="123" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:27">
+    <row r="125" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:27">
+    <row r="126" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -2677,8 +3171,21 @@
       <c r="Y126" s="1"/>
       <c r="Z126" s="1"/>
       <c r="AA126" s="1"/>
-    </row>
-    <row r="127" spans="1:27">
+      <c r="AB126" s="1"/>
+      <c r="AC126" s="1"/>
+      <c r="AD126" s="1"/>
+      <c r="AE126" s="1"/>
+      <c r="AF126" s="1"/>
+      <c r="AG126" s="1"/>
+      <c r="AH126" s="1"/>
+      <c r="AI126" s="1"/>
+      <c r="AJ126" s="1"/>
+      <c r="AK126" s="1"/>
+      <c r="AL126" s="1"/>
+      <c r="AM126" s="1"/>
+      <c r="AN126" s="1"/>
+    </row>
+    <row r="127" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -2706,8 +3213,21 @@
       <c r="Y127" s="1"/>
       <c r="Z127" s="1"/>
       <c r="AA127" s="1"/>
-    </row>
-    <row r="128" spans="1:27">
+      <c r="AB127" s="1"/>
+      <c r="AC127" s="1"/>
+      <c r="AD127" s="1"/>
+      <c r="AE127" s="1"/>
+      <c r="AF127" s="1"/>
+      <c r="AG127" s="1"/>
+      <c r="AH127" s="1"/>
+      <c r="AI127" s="1"/>
+      <c r="AJ127" s="1"/>
+      <c r="AK127" s="1"/>
+      <c r="AL127" s="1"/>
+      <c r="AM127" s="1"/>
+      <c r="AN127" s="1"/>
+    </row>
+    <row r="128" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -2735,8 +3255,21 @@
       <c r="Y128" s="1"/>
       <c r="Z128" s="1"/>
       <c r="AA128" s="1"/>
-    </row>
-    <row r="129" spans="1:27">
+      <c r="AB128" s="1"/>
+      <c r="AC128" s="1"/>
+      <c r="AD128" s="1"/>
+      <c r="AE128" s="1"/>
+      <c r="AF128" s="1"/>
+      <c r="AG128" s="1"/>
+      <c r="AH128" s="1"/>
+      <c r="AI128" s="1"/>
+      <c r="AJ128" s="1"/>
+      <c r="AK128" s="1"/>
+      <c r="AL128" s="1"/>
+      <c r="AM128" s="1"/>
+      <c r="AN128" s="1"/>
+    </row>
+    <row r="129" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -2764,8 +3297,21 @@
       <c r="Y129" s="1"/>
       <c r="Z129" s="1"/>
       <c r="AA129" s="1"/>
-    </row>
-    <row r="130" spans="1:27">
+      <c r="AB129" s="1"/>
+      <c r="AC129" s="1"/>
+      <c r="AD129" s="1"/>
+      <c r="AE129" s="1"/>
+      <c r="AF129" s="1"/>
+      <c r="AG129" s="1"/>
+      <c r="AH129" s="1"/>
+      <c r="AI129" s="1"/>
+      <c r="AJ129" s="1"/>
+      <c r="AK129" s="1"/>
+      <c r="AL129" s="1"/>
+      <c r="AM129" s="1"/>
+      <c r="AN129" s="1"/>
+    </row>
+    <row r="130" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -2793,8 +3339,21 @@
       <c r="Y130" s="1"/>
       <c r="Z130" s="1"/>
       <c r="AA130" s="1"/>
-    </row>
-    <row r="131" spans="1:27">
+      <c r="AB130" s="1"/>
+      <c r="AC130" s="1"/>
+      <c r="AD130" s="1"/>
+      <c r="AE130" s="1"/>
+      <c r="AF130" s="1"/>
+      <c r="AG130" s="1"/>
+      <c r="AH130" s="1"/>
+      <c r="AI130" s="1"/>
+      <c r="AJ130" s="1"/>
+      <c r="AK130" s="1"/>
+      <c r="AL130" s="1"/>
+      <c r="AM130" s="1"/>
+      <c r="AN130" s="1"/>
+    </row>
+    <row r="131" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -2822,8 +3381,21 @@
       <c r="Y131" s="1"/>
       <c r="Z131" s="1"/>
       <c r="AA131" s="1"/>
-    </row>
-    <row r="132" spans="1:27">
+      <c r="AB131" s="1"/>
+      <c r="AC131" s="1"/>
+      <c r="AD131" s="1"/>
+      <c r="AE131" s="1"/>
+      <c r="AF131" s="1"/>
+      <c r="AG131" s="1"/>
+      <c r="AH131" s="1"/>
+      <c r="AI131" s="1"/>
+      <c r="AJ131" s="1"/>
+      <c r="AK131" s="1"/>
+      <c r="AL131" s="1"/>
+      <c r="AM131" s="1"/>
+      <c r="AN131" s="1"/>
+    </row>
+    <row r="132" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -2851,8 +3423,21 @@
       <c r="Y132" s="1"/>
       <c r="Z132" s="1"/>
       <c r="AA132" s="1"/>
-    </row>
-    <row r="133" spans="1:27">
+      <c r="AB132" s="1"/>
+      <c r="AC132" s="1"/>
+      <c r="AD132" s="1"/>
+      <c r="AE132" s="1"/>
+      <c r="AF132" s="1"/>
+      <c r="AG132" s="1"/>
+      <c r="AH132" s="1"/>
+      <c r="AI132" s="1"/>
+      <c r="AJ132" s="1"/>
+      <c r="AK132" s="1"/>
+      <c r="AL132" s="1"/>
+      <c r="AM132" s="1"/>
+      <c r="AN132" s="1"/>
+    </row>
+    <row r="133" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -2880,8 +3465,21 @@
       <c r="Y133" s="1"/>
       <c r="Z133" s="1"/>
       <c r="AA133" s="1"/>
-    </row>
-    <row r="134" spans="1:27">
+      <c r="AB133" s="1"/>
+      <c r="AC133" s="1"/>
+      <c r="AD133" s="1"/>
+      <c r="AE133" s="1"/>
+      <c r="AF133" s="1"/>
+      <c r="AG133" s="1"/>
+      <c r="AH133" s="1"/>
+      <c r="AI133" s="1"/>
+      <c r="AJ133" s="1"/>
+      <c r="AK133" s="1"/>
+      <c r="AL133" s="1"/>
+      <c r="AM133" s="1"/>
+      <c r="AN133" s="1"/>
+    </row>
+    <row r="134" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -2909,8 +3507,21 @@
       <c r="Y134" s="1"/>
       <c r="Z134" s="1"/>
       <c r="AA134" s="1"/>
-    </row>
-    <row r="135" spans="1:27">
+      <c r="AB134" s="1"/>
+      <c r="AC134" s="1"/>
+      <c r="AD134" s="1"/>
+      <c r="AE134" s="1"/>
+      <c r="AF134" s="1"/>
+      <c r="AG134" s="1"/>
+      <c r="AH134" s="1"/>
+      <c r="AI134" s="1"/>
+      <c r="AJ134" s="1"/>
+      <c r="AK134" s="1"/>
+      <c r="AL134" s="1"/>
+      <c r="AM134" s="1"/>
+      <c r="AN134" s="1"/>
+    </row>
+    <row r="135" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -2938,8 +3549,21 @@
       <c r="Y135" s="1"/>
       <c r="Z135" s="1"/>
       <c r="AA135" s="1"/>
-    </row>
-    <row r="136" spans="1:27">
+      <c r="AB135" s="1"/>
+      <c r="AC135" s="1"/>
+      <c r="AD135" s="1"/>
+      <c r="AE135" s="1"/>
+      <c r="AF135" s="1"/>
+      <c r="AG135" s="1"/>
+      <c r="AH135" s="1"/>
+      <c r="AI135" s="1"/>
+      <c r="AJ135" s="1"/>
+      <c r="AK135" s="1"/>
+      <c r="AL135" s="1"/>
+      <c r="AM135" s="1"/>
+      <c r="AN135" s="1"/>
+    </row>
+    <row r="136" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -2967,8 +3591,21 @@
       <c r="Y136" s="1"/>
       <c r="Z136" s="1"/>
       <c r="AA136" s="1"/>
-    </row>
-    <row r="137" spans="1:27">
+      <c r="AB136" s="1"/>
+      <c r="AC136" s="1"/>
+      <c r="AD136" s="1"/>
+      <c r="AE136" s="1"/>
+      <c r="AF136" s="1"/>
+      <c r="AG136" s="1"/>
+      <c r="AH136" s="1"/>
+      <c r="AI136" s="1"/>
+      <c r="AJ136" s="1"/>
+      <c r="AK136" s="1"/>
+      <c r="AL136" s="1"/>
+      <c r="AM136" s="1"/>
+      <c r="AN136" s="1"/>
+    </row>
+    <row r="137" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -2996,8 +3633,21 @@
       <c r="Y137" s="1"/>
       <c r="Z137" s="1"/>
       <c r="AA137" s="1"/>
-    </row>
-    <row r="138" spans="1:27">
+      <c r="AB137" s="1"/>
+      <c r="AC137" s="1"/>
+      <c r="AD137" s="1"/>
+      <c r="AE137" s="1"/>
+      <c r="AF137" s="1"/>
+      <c r="AG137" s="1"/>
+      <c r="AH137" s="1"/>
+      <c r="AI137" s="1"/>
+      <c r="AJ137" s="1"/>
+      <c r="AK137" s="1"/>
+      <c r="AL137" s="1"/>
+      <c r="AM137" s="1"/>
+      <c r="AN137" s="1"/>
+    </row>
+    <row r="138" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3025,8 +3675,21 @@
       <c r="Y138" s="1"/>
       <c r="Z138" s="1"/>
       <c r="AA138" s="1"/>
-    </row>
-    <row r="139" spans="1:27">
+      <c r="AB138" s="1"/>
+      <c r="AC138" s="1"/>
+      <c r="AD138" s="1"/>
+      <c r="AE138" s="1"/>
+      <c r="AF138" s="1"/>
+      <c r="AG138" s="1"/>
+      <c r="AH138" s="1"/>
+      <c r="AI138" s="1"/>
+      <c r="AJ138" s="1"/>
+      <c r="AK138" s="1"/>
+      <c r="AL138" s="1"/>
+      <c r="AM138" s="1"/>
+      <c r="AN138" s="1"/>
+    </row>
+    <row r="139" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3054,8 +3717,21 @@
       <c r="Y139" s="1"/>
       <c r="Z139" s="1"/>
       <c r="AA139" s="1"/>
-    </row>
-    <row r="140" spans="1:27">
+      <c r="AB139" s="1"/>
+      <c r="AC139" s="1"/>
+      <c r="AD139" s="1"/>
+      <c r="AE139" s="1"/>
+      <c r="AF139" s="1"/>
+      <c r="AG139" s="1"/>
+      <c r="AH139" s="1"/>
+      <c r="AI139" s="1"/>
+      <c r="AJ139" s="1"/>
+      <c r="AK139" s="1"/>
+      <c r="AL139" s="1"/>
+      <c r="AM139" s="1"/>
+      <c r="AN139" s="1"/>
+    </row>
+    <row r="140" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>9</v>
       </c>
@@ -3089,8 +3765,21 @@
       <c r="Y140" s="1"/>
       <c r="Z140" s="1"/>
       <c r="AA140" s="1"/>
-    </row>
-    <row r="141" spans="1:27">
+      <c r="AB140" s="1"/>
+      <c r="AC140" s="1"/>
+      <c r="AD140" s="1"/>
+      <c r="AE140" s="1"/>
+      <c r="AF140" s="1"/>
+      <c r="AG140" s="1"/>
+      <c r="AH140" s="1"/>
+      <c r="AI140" s="1"/>
+      <c r="AJ140" s="1"/>
+      <c r="AK140" s="1"/>
+      <c r="AL140" s="1"/>
+      <c r="AM140" s="1"/>
+      <c r="AN140" s="1"/>
+    </row>
+    <row r="141" spans="1:40" x14ac:dyDescent="0.2">
       <c r="R141" s="1"/>
       <c r="S141" s="1"/>
       <c r="T141" s="1"/>
@@ -3101,8 +3790,21 @@
       <c r="Y141" s="1"/>
       <c r="Z141" s="1"/>
       <c r="AA141" s="1"/>
-    </row>
-    <row r="142" spans="1:27">
+      <c r="AB141" s="1"/>
+      <c r="AC141" s="1"/>
+      <c r="AD141" s="1"/>
+      <c r="AE141" s="1"/>
+      <c r="AF141" s="1"/>
+      <c r="AG141" s="1"/>
+      <c r="AH141" s="1"/>
+      <c r="AI141" s="1"/>
+      <c r="AJ141" s="1"/>
+      <c r="AK141" s="1"/>
+      <c r="AL141" s="1"/>
+      <c r="AM141" s="1"/>
+      <c r="AN141" s="1"/>
+    </row>
+    <row r="142" spans="1:40" x14ac:dyDescent="0.2">
       <c r="R142" s="1"/>
       <c r="S142" s="1"/>
       <c r="T142" s="1"/>
@@ -3113,8 +3815,21 @@
       <c r="Y142" s="1"/>
       <c r="Z142" s="1"/>
       <c r="AA142" s="1"/>
-    </row>
-    <row r="143" spans="1:27">
+      <c r="AB142" s="1"/>
+      <c r="AC142" s="1"/>
+      <c r="AD142" s="1"/>
+      <c r="AE142" s="1"/>
+      <c r="AF142" s="1"/>
+      <c r="AG142" s="1"/>
+      <c r="AH142" s="1"/>
+      <c r="AI142" s="1"/>
+      <c r="AJ142" s="1"/>
+      <c r="AK142" s="1"/>
+      <c r="AL142" s="1"/>
+      <c r="AM142" s="1"/>
+      <c r="AN142" s="1"/>
+    </row>
+    <row r="143" spans="1:40" x14ac:dyDescent="0.2">
       <c r="R143" s="1"/>
       <c r="S143" s="1"/>
       <c r="T143" s="1"/>
@@ -3125,8 +3840,21 @@
       <c r="Y143" s="1"/>
       <c r="Z143" s="1"/>
       <c r="AA143" s="1"/>
-    </row>
-    <row r="144" spans="1:27">
+      <c r="AB143" s="1"/>
+      <c r="AC143" s="1"/>
+      <c r="AD143" s="1"/>
+      <c r="AE143" s="1"/>
+      <c r="AF143" s="1"/>
+      <c r="AG143" s="1"/>
+      <c r="AH143" s="1"/>
+      <c r="AI143" s="1"/>
+      <c r="AJ143" s="1"/>
+      <c r="AK143" s="1"/>
+      <c r="AL143" s="1"/>
+      <c r="AM143" s="1"/>
+      <c r="AN143" s="1"/>
+    </row>
+    <row r="144" spans="1:40" x14ac:dyDescent="0.2">
       <c r="R144" s="1"/>
       <c r="S144" s="1"/>
       <c r="T144" s="1"/>
@@ -3137,8 +3865,21 @@
       <c r="Y144" s="1"/>
       <c r="Z144" s="1"/>
       <c r="AA144" s="1"/>
-    </row>
-    <row r="145" spans="18:27">
+      <c r="AB144" s="1"/>
+      <c r="AC144" s="1"/>
+      <c r="AD144" s="1"/>
+      <c r="AE144" s="1"/>
+      <c r="AF144" s="1"/>
+      <c r="AG144" s="1"/>
+      <c r="AH144" s="1"/>
+      <c r="AI144" s="1"/>
+      <c r="AJ144" s="1"/>
+      <c r="AK144" s="1"/>
+      <c r="AL144" s="1"/>
+      <c r="AM144" s="1"/>
+      <c r="AN144" s="1"/>
+    </row>
+    <row r="145" spans="18:40" x14ac:dyDescent="0.2">
       <c r="R145" s="1"/>
       <c r="S145" s="1"/>
       <c r="T145" s="1"/>
@@ -3149,8 +3890,21 @@
       <c r="Y145" s="1"/>
       <c r="Z145" s="1"/>
       <c r="AA145" s="1"/>
-    </row>
-    <row r="146" spans="18:27">
+      <c r="AB145" s="1"/>
+      <c r="AC145" s="1"/>
+      <c r="AD145" s="1"/>
+      <c r="AE145" s="1"/>
+      <c r="AF145" s="1"/>
+      <c r="AG145" s="1"/>
+      <c r="AH145" s="1"/>
+      <c r="AI145" s="1"/>
+      <c r="AJ145" s="1"/>
+      <c r="AK145" s="1"/>
+      <c r="AL145" s="1"/>
+      <c r="AM145" s="1"/>
+      <c r="AN145" s="1"/>
+    </row>
+    <row r="146" spans="18:40" x14ac:dyDescent="0.2">
       <c r="R146" s="1"/>
       <c r="S146" s="1"/>
       <c r="T146" s="1"/>
@@ -3161,8 +3915,21 @@
       <c r="Y146" s="1"/>
       <c r="Z146" s="1"/>
       <c r="AA146" s="1"/>
-    </row>
-    <row r="147" spans="18:27">
+      <c r="AB146" s="1"/>
+      <c r="AC146" s="1"/>
+      <c r="AD146" s="1"/>
+      <c r="AE146" s="1"/>
+      <c r="AF146" s="1"/>
+      <c r="AG146" s="1"/>
+      <c r="AH146" s="1"/>
+      <c r="AI146" s="1"/>
+      <c r="AJ146" s="1"/>
+      <c r="AK146" s="1"/>
+      <c r="AL146" s="1"/>
+      <c r="AM146" s="1"/>
+      <c r="AN146" s="1"/>
+    </row>
+    <row r="147" spans="18:40" x14ac:dyDescent="0.2">
       <c r="R147" s="1"/>
       <c r="S147" s="1"/>
       <c r="T147" s="1"/>
@@ -3173,8 +3940,21 @@
       <c r="Y147" s="1"/>
       <c r="Z147" s="1"/>
       <c r="AA147" s="1"/>
-    </row>
-    <row r="148" spans="18:27">
+      <c r="AB147" s="1"/>
+      <c r="AC147" s="1"/>
+      <c r="AD147" s="1"/>
+      <c r="AE147" s="1"/>
+      <c r="AF147" s="1"/>
+      <c r="AG147" s="1"/>
+      <c r="AH147" s="1"/>
+      <c r="AI147" s="1"/>
+      <c r="AJ147" s="1"/>
+      <c r="AK147" s="1"/>
+      <c r="AL147" s="1"/>
+      <c r="AM147" s="1"/>
+      <c r="AN147" s="1"/>
+    </row>
+    <row r="148" spans="18:40" x14ac:dyDescent="0.2">
       <c r="R148" s="1"/>
       <c r="S148" s="1"/>
       <c r="T148" s="1"/>
@@ -3185,8 +3965,21 @@
       <c r="Y148" s="1"/>
       <c r="Z148" s="1"/>
       <c r="AA148" s="1"/>
-    </row>
-    <row r="149" spans="18:27">
+      <c r="AB148" s="1"/>
+      <c r="AC148" s="1"/>
+      <c r="AD148" s="1"/>
+      <c r="AE148" s="1"/>
+      <c r="AF148" s="1"/>
+      <c r="AG148" s="1"/>
+      <c r="AH148" s="1"/>
+      <c r="AI148" s="1"/>
+      <c r="AJ148" s="1"/>
+      <c r="AK148" s="1"/>
+      <c r="AL148" s="1"/>
+      <c r="AM148" s="1"/>
+      <c r="AN148" s="1"/>
+    </row>
+    <row r="149" spans="18:40" x14ac:dyDescent="0.2">
       <c r="R149" s="1"/>
       <c r="S149" s="1"/>
       <c r="T149" s="1"/>
@@ -3197,8 +3990,21 @@
       <c r="Y149" s="1"/>
       <c r="Z149" s="1"/>
       <c r="AA149" s="1"/>
-    </row>
-    <row r="150" spans="18:27">
+      <c r="AB149" s="1"/>
+      <c r="AC149" s="1"/>
+      <c r="AD149" s="1"/>
+      <c r="AE149" s="1"/>
+      <c r="AF149" s="1"/>
+      <c r="AG149" s="1"/>
+      <c r="AH149" s="1"/>
+      <c r="AI149" s="1"/>
+      <c r="AJ149" s="1"/>
+      <c r="AK149" s="1"/>
+      <c r="AL149" s="1"/>
+      <c r="AM149" s="1"/>
+      <c r="AN149" s="1"/>
+    </row>
+    <row r="150" spans="18:40" x14ac:dyDescent="0.2">
       <c r="R150" s="1"/>
       <c r="S150" s="1"/>
       <c r="T150" s="1"/>
@@ -3209,8 +4015,21 @@
       <c r="Y150" s="1"/>
       <c r="Z150" s="1"/>
       <c r="AA150" s="1"/>
-    </row>
-    <row r="151" spans="18:27">
+      <c r="AB150" s="1"/>
+      <c r="AC150" s="1"/>
+      <c r="AD150" s="1"/>
+      <c r="AE150" s="1"/>
+      <c r="AF150" s="1"/>
+      <c r="AG150" s="1"/>
+      <c r="AH150" s="1"/>
+      <c r="AI150" s="1"/>
+      <c r="AJ150" s="1"/>
+      <c r="AK150" s="1"/>
+      <c r="AL150" s="1"/>
+      <c r="AM150" s="1"/>
+      <c r="AN150" s="1"/>
+    </row>
+    <row r="151" spans="18:40" x14ac:dyDescent="0.2">
       <c r="R151" s="1"/>
       <c r="S151" s="1"/>
       <c r="T151" s="1"/>
@@ -3221,8 +4040,21 @@
       <c r="Y151" s="1"/>
       <c r="Z151" s="1"/>
       <c r="AA151" s="1"/>
-    </row>
-    <row r="152" spans="18:27">
+      <c r="AB151" s="1"/>
+      <c r="AC151" s="1"/>
+      <c r="AD151" s="1"/>
+      <c r="AE151" s="1"/>
+      <c r="AF151" s="1"/>
+      <c r="AG151" s="1"/>
+      <c r="AH151" s="1"/>
+      <c r="AI151" s="1"/>
+      <c r="AJ151" s="1"/>
+      <c r="AK151" s="1"/>
+      <c r="AL151" s="1"/>
+      <c r="AM151" s="1"/>
+      <c r="AN151" s="1"/>
+    </row>
+    <row r="152" spans="18:40" x14ac:dyDescent="0.2">
       <c r="R152" s="1"/>
       <c r="S152" s="1"/>
       <c r="T152" s="1"/>
@@ -3233,8 +4065,21 @@
       <c r="Y152" s="1"/>
       <c r="Z152" s="1"/>
       <c r="AA152" s="1"/>
-    </row>
-    <row r="153" spans="18:27">
+      <c r="AB152" s="1"/>
+      <c r="AC152" s="1"/>
+      <c r="AD152" s="1"/>
+      <c r="AE152" s="1"/>
+      <c r="AF152" s="1"/>
+      <c r="AG152" s="1"/>
+      <c r="AH152" s="1"/>
+      <c r="AI152" s="1"/>
+      <c r="AJ152" s="1"/>
+      <c r="AK152" s="1"/>
+      <c r="AL152" s="1"/>
+      <c r="AM152" s="1"/>
+      <c r="AN152" s="1"/>
+    </row>
+    <row r="153" spans="18:40" x14ac:dyDescent="0.2">
       <c r="R153" s="1"/>
       <c r="S153" s="1"/>
       <c r="T153" s="1"/>
@@ -3245,6 +4090,70 @@
       <c r="Y153" s="1"/>
       <c r="Z153" s="1"/>
       <c r="AA153" s="1"/>
+      <c r="AB153" s="1"/>
+      <c r="AC153" s="1"/>
+      <c r="AD153" s="1"/>
+      <c r="AE153" s="1"/>
+      <c r="AF153" s="1"/>
+      <c r="AG153" s="1"/>
+      <c r="AH153" s="1"/>
+      <c r="AI153" s="1"/>
+      <c r="AJ153" s="1"/>
+      <c r="AK153" s="1"/>
+      <c r="AL153" s="1"/>
+      <c r="AM153" s="1"/>
+      <c r="AN153" s="1"/>
+    </row>
+    <row r="154" spans="18:40" x14ac:dyDescent="0.2">
+      <c r="Z154" s="1"/>
+      <c r="AA154" s="1"/>
+      <c r="AB154" s="1"/>
+      <c r="AC154" s="1"/>
+      <c r="AD154" s="1"/>
+      <c r="AE154" s="1"/>
+      <c r="AF154" s="1"/>
+      <c r="AG154" s="1"/>
+      <c r="AH154" s="1"/>
+      <c r="AI154" s="1"/>
+      <c r="AJ154" s="1"/>
+      <c r="AK154" s="1"/>
+      <c r="AL154" s="1"/>
+      <c r="AM154" s="1"/>
+      <c r="AN154" s="1"/>
+    </row>
+    <row r="155" spans="18:40" x14ac:dyDescent="0.2">
+      <c r="Z155" s="1"/>
+      <c r="AA155" s="1"/>
+      <c r="AB155" s="1"/>
+      <c r="AC155" s="1"/>
+      <c r="AD155" s="1"/>
+      <c r="AE155" s="1"/>
+      <c r="AF155" s="1"/>
+      <c r="AG155" s="1"/>
+      <c r="AH155" s="1"/>
+      <c r="AI155" s="1"/>
+      <c r="AJ155" s="1"/>
+      <c r="AK155" s="1"/>
+      <c r="AL155" s="1"/>
+      <c r="AM155" s="1"/>
+      <c r="AN155" s="1"/>
+    </row>
+    <row r="156" spans="18:40" x14ac:dyDescent="0.2">
+      <c r="Z156" s="1"/>
+      <c r="AA156" s="1"/>
+      <c r="AB156" s="1"/>
+      <c r="AC156" s="1"/>
+      <c r="AD156" s="1"/>
+      <c r="AE156" s="1"/>
+      <c r="AF156" s="1"/>
+      <c r="AG156" s="1"/>
+      <c r="AH156" s="1"/>
+      <c r="AI156" s="1"/>
+      <c r="AJ156" s="1"/>
+      <c r="AK156" s="1"/>
+      <c r="AL156" s="1"/>
+      <c r="AM156" s="1"/>
+      <c r="AN156" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bugfix for xaxis being wrong! Silly mistake by Eghbal!
</commit_message>
<xml_diff>
--- a/training_csv_overview/overview_traindyn_favorites.xlsx
+++ b/training_csv_overview/overview_traindyn_favorites.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gt/Documents/GitHub/neural_manifolds/training_csv_overview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eghbalhosseini/MyCodes/neural_manifolds/training_csv_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13A90E2-470E-6B46-B5F8-DFD8E55ED5C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3FC5E6-1A8C-9041-93D8-4295567BCC6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20900" xr2:uid="{57D70428-E33C-FB43-9F81-CF825DE71854}"/>
+    <workbookView xWindow="-36520" yWindow="2100" windowWidth="34600" windowHeight="21100" xr2:uid="{57D70428-E33C-FB43-9F81-CF825DE71854}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>lr 0.0005, momentum 0.5, gaussian std 0.0001, batch size 32, 20 epochs</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t xml:space="preserve">capacity in layer 1 - great for upper hier? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate of change in the distance for different layers </t>
   </si>
 </sst>
 </file>
@@ -552,15 +555,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
+      <xdr:colOff>63500</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
+      <xdr:colOff>482600</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -583,7 +586,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5194300" y="9766300"/>
+          <a:off x="5016500" y="9753600"/>
           <a:ext cx="4546600" cy="2044700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -640,22 +643,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>787399</xdr:colOff>
+      <xdr:colOff>808182</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>144319</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>242812</xdr:colOff>
+      <xdr:colOff>90207</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>72159</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
+        <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0363862-B1D3-B146-AB75-D15DD9BC6149}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3775AAD8-BCC7-6444-9860-E1BA4F0C0293}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -671,8 +674,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11518899" y="3797300"/>
-          <a:ext cx="8535913" cy="5308600"/>
+          <a:off x="11502159" y="3781137"/>
+          <a:ext cx="8330775" cy="5181022"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -684,22 +687,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>72160</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>158749</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
+      <xdr:colOff>808182</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>34324</xdr:rowOff>
+      <xdr:rowOff>40174</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
+        <xdr:cNvPr id="16" name="Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96274132-F21A-0149-A49A-82D6EBBF3A87}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF3FF1D0-0F38-F64A-A4F4-67E1A5389CA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -715,8 +718,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20193000" y="3098800"/>
-          <a:ext cx="9372600" cy="6079524"/>
+          <a:off x="19814887" y="2785340"/>
+          <a:ext cx="9784772" cy="6346879"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -727,23 +730,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>57727</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>216406</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>118285</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17">
+        <xdr:cNvPr id="17" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD73F178-A670-0242-90C5-AD385C0F984C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9ACD35B-5D45-3F46-A12A-853E7946D9A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -759,8 +762,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11544300" y="9398000"/>
-          <a:ext cx="8484106" cy="5334000"/>
+          <a:off x="11574318" y="9294091"/>
+          <a:ext cx="8286694" cy="5209886"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -772,22 +775,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:colOff>115453</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>165099</xdr:rowOff>
+      <xdr:rowOff>43295</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>99197</xdr:rowOff>
+      <xdr:colOff>721591</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>42515</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19">
+        <xdr:cNvPr id="19" name="Picture 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4D8664E-6C49-334E-8807-4B00BABF7823}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEFC9A1D-7EA4-B84E-AA37-9E85DAE3CC30}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -803,8 +806,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20307300" y="9309099"/>
-          <a:ext cx="9296400" cy="6030098"/>
+          <a:off x="19858180" y="9135340"/>
+          <a:ext cx="9654888" cy="6262630"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -815,23 +818,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>596212</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>678297</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>165431</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>517528</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>120135</xdr:rowOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>432955</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>194519</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 21">
+        <xdr:cNvPr id="21" name="Picture 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DF593B8-A035-4940-998B-E55C48DDE75A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22F63B38-BB1C-CB42-9456-C8AF1E370336}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -847,8 +850,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13776753" y="25715097"/>
-          <a:ext cx="8982937" cy="5708822"/>
+          <a:off x="22888865" y="25219067"/>
+          <a:ext cx="9626022" cy="6292497"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -859,23 +862,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>669324</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>678295</xdr:colOff>
       <xdr:row>125</xdr:row>
-      <xdr:rowOff>34323</xdr:rowOff>
+      <xdr:rowOff>57727</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>629176</xdr:colOff>
-      <xdr:row>156</xdr:row>
-      <xdr:rowOff>85809</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>300956</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>28864</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 22">
+        <xdr:cNvPr id="24" name="Picture 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54535780-9A73-5740-A2DD-92E92311E67D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22681494-5A66-294E-9AFB-CCA97030E218}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -891,8 +894,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22911486" y="25777566"/>
-          <a:ext cx="9845258" cy="6435811"/>
+          <a:off x="13840113" y="25313409"/>
+          <a:ext cx="8671411" cy="5426364"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1203,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B08E62D4-B6AA-6D4B-AA5A-6F10267A87F4}">
   <dimension ref="A3:AN156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D116" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="U159" sqref="U159"/>
+    <sheetView tabSelected="1" topLeftCell="J18" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="Z121" sqref="Z121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3088,6 +3091,9 @@
       <c r="AK73" s="1"/>
     </row>
     <row r="74" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="P74" t="s">
+        <v>19</v>
+      </c>
       <c r="Y74" s="1"/>
       <c r="Z74" s="1"/>
       <c r="AA74" s="1"/>

</xml_diff>